<commit_message>
Adding labels/technologyLabel to output Excel file in createFileString()
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInput.xlsx
+++ b/inputData/VencoPy_scalarInput.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68BD03-E3B1-4FD3-8D8A-8FD490D2D35E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE1219-632D-41C9-B940-E910126D1E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs of Model" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -55,9 +55,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Minimum daily mileage</t>
-  </si>
-  <si>
     <t>File Info</t>
   </si>
   <si>
@@ -73,37 +70,40 @@
     <t>VencoPy Input Assumptions</t>
   </si>
   <si>
-    <t>Electric consumption NEFZ</t>
-  </si>
-  <si>
-    <t>Fuel consumption NEFZ</t>
-  </si>
-  <si>
-    <t>Electric consumption Artemis</t>
-  </si>
-  <si>
-    <t>Fuel consumption Artemis</t>
-  </si>
-  <si>
-    <t>Maximum SOC</t>
-  </si>
-  <si>
-    <t>Minimum SOC</t>
-  </si>
-  <si>
-    <t>Rated power of charging column</t>
-  </si>
-  <si>
-    <t>Is BEV?</t>
-  </si>
-  <si>
-    <t>Battery capacity</t>
-  </si>
-  <si>
-    <t>16.04.2020</t>
-  </si>
-  <si>
     <t>Originally from Diego Luca de Tena (DLR-TT) based on the tables from Bernd Propfe (DLR-FK), updated by Niklas Wulff (DLR-TT) as input sheet for VencoPy. Licensed under BSD 3-Clause</t>
+  </si>
+  <si>
+    <t>06.10.2020</t>
+  </si>
+  <si>
+    <t>Minimum_daily_mileage</t>
+  </si>
+  <si>
+    <t>Battery_capacity</t>
+  </si>
+  <si>
+    <t>Electric_consumption_NEFZ</t>
+  </si>
+  <si>
+    <t>Fuel_consumption_NEFZ</t>
+  </si>
+  <si>
+    <t>Electric_consumption_Artemis</t>
+  </si>
+  <si>
+    <t>Fuel_consumption_Artemis</t>
+  </si>
+  <si>
+    <t>Maximum_SOC</t>
+  </si>
+  <si>
+    <t>Minimum_SOC</t>
+  </si>
+  <si>
+    <t>Rated_power_of_charging_column</t>
+  </si>
+  <si>
+    <t>Is_BEV?</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -560,23 +560,23 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -584,7 +584,7 @@
     </row>
     <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="3"/>
@@ -622,7 +622,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="9">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -656,10 +656,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10">
-        <v>8.5</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="10">
         <v>1</v>
@@ -685,10 +685,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="10">
         <v>19</v>
-      </c>
-      <c r="B11" s="10">
-        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B13" s="11">
         <v>0.97</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11">
         <v>0.03</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8">
-        <v>3.7</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -740,13 +740,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added some standalone functionailities of Evaluator, changed labels in globalConfig, updated schema
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInput.xlsx
+++ b/inputData/VencoPy_scalarInput.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE1219-632D-41C9-B940-E910126D1E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55297B9A-DD2D-43F7-B32E-8F53DF3FE7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs of Model" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -547,7 +547,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -642,7 +642,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="9">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="8">
-        <v>11</v>
+        <v>3.6</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Minor changes for bugfixing on gridmodeling branch
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInput.xlsx
+++ b/inputData/VencoPy_scalarInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55297B9A-DD2D-43F7-B32E-8F53DF3FE7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10213DDF-117A-4EEF-9D4E-3DD98BA53FA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,7 +732,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="8">
-        <v>3.6</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>

</xml_diff>